<commit_message>
change format of slimMapper...Function.xlsx
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/proteinevoutk20@301 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/pkg/Result/slimMapperResult-Function.xlsx
+++ b/pkg/Result/slimMapperResult-Function.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="24880" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="51240" yWindow="-440" windowWidth="24880" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="slimMapperResult-Function.xls" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="160">
   <si>
     <t>GOID</t>
   </si>
@@ -45,9 +45,6 @@
     <t>1970 of 6334 genes, 31.1%</t>
   </si>
   <si>
-    <t>YBR056W,TOS1,CWH43,ARX1,BCP1,ICE2,FRA1,YLR253W,YML096W,YNL155W,RPA49,SEC21,EMW1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ligase activity</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>185 of 6334 genes, 2.9%</t>
   </si>
   <si>
-    <t>CDC34,AIM10,VAS1,DED81,TRL1,TUL1,ADE12,GSH2,WRS1,MSD1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> DNA binding</t>
   </si>
   <si>
@@ -69,18 +63,12 @@
     <t>376 of 6334 genes, 5.9%</t>
   </si>
   <si>
-    <t>RFA1,RAD23,PRI1,RFC2,BAS1,PMS1,ADE12,CTR9,HST3</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ATPase activity</t>
   </si>
   <si>
     <t>236 of 6334 genes, 3.7%</t>
   </si>
   <si>
-    <t>ATP3,DBP10,CDC48,FAL1,RFC2,NPA3,HSC82,PMS1,DBP6</t>
-  </si>
-  <si>
     <t xml:space="preserve"> oxidoreductase activity</t>
   </si>
   <si>
@@ -90,36 +78,24 @@
     <t>276 of 6334 genes, 4.4%</t>
   </si>
   <si>
-    <t>GDH2,ERG26,POX1,KGD1,ERG5,ARA2</t>
-  </si>
-  <si>
     <t xml:space="preserve"> transferase activity, transferring acyl groups</t>
   </si>
   <si>
     <t>119 of 6334 genes, 1.9%</t>
   </si>
   <si>
-    <t>NGG1,TGL4,LEU4,LRO1,ERG10,TAZ1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> peptidase activity</t>
   </si>
   <si>
     <t>137 of 6334 genes, 2.2%</t>
   </si>
   <si>
-    <t>MAP2,DUG1,STE24,STE23,NMA111,MCA1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> transmembrane transporter activity</t>
   </si>
   <si>
     <t>314 of 6334 genes, 5%</t>
   </si>
   <si>
-    <t>FLC2,ATP3,VRG4,AVT7,OAC1,TOM40</t>
-  </si>
-  <si>
     <t xml:space="preserve"> kinase activity</t>
   </si>
   <si>
@@ -129,36 +105,24 @@
     <t>199 of 6334 genes, 3.1%</t>
   </si>
   <si>
-    <t>CAB1,HXK2,XKS1,TRL1,LSB6</t>
-  </si>
-  <si>
     <t xml:space="preserve"> protein binding transcription factor activity</t>
   </si>
   <si>
     <t>132 of 6334 genes, 2.1%</t>
   </si>
   <si>
-    <t>NGG1,SSN2,TFG2,BAS1,CTR9</t>
-  </si>
-  <si>
     <t xml:space="preserve"> methyltransferase activity</t>
   </si>
   <si>
     <t>92 of 6334 genes, 1.5%</t>
   </si>
   <si>
-    <t>SPB1,RMT2,IME4,COQ5,GCD10</t>
-  </si>
-  <si>
     <t xml:space="preserve"> structural molecule activity</t>
   </si>
   <si>
     <t>356 of 6334 genes, 5.6%</t>
   </si>
   <si>
-    <t>TAF5,NUP84,SEC31,PET123,MEX67</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ion binding</t>
   </si>
   <si>
@@ -168,9 +132,6 @@
     <t>126 of 6334 genes, 2%</t>
   </si>
   <si>
-    <t>YLF2,EXO70,PMS1,SSE1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> helicase activity</t>
   </si>
   <si>
@@ -180,54 +141,36 @@
     <t>85 of 6334 genes, 1.3%</t>
   </si>
   <si>
-    <t>DBP10,FAL1,DBP6</t>
-  </si>
-  <si>
     <t xml:space="preserve"> small conjugating protein binding</t>
   </si>
   <si>
     <t>43 of 6334 genes, 0.7%</t>
   </si>
   <si>
-    <t>TAF5,CDC48,RAD23</t>
-  </si>
-  <si>
     <t xml:space="preserve"> hydrolase activity, acting on carbon-nitrogen (but not peptide) bonds</t>
   </si>
   <si>
     <t>61 of 6334 genes, 1%</t>
   </si>
   <si>
-    <t>GUD1,RAD23,HST3</t>
-  </si>
-  <si>
     <t xml:space="preserve"> transferase activity, transferring glycosyl groups</t>
   </si>
   <si>
     <t>100 of 6334 genes, 1.6%</t>
   </si>
   <si>
-    <t>ALG14,ALG1,TPS1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> phosphatase activity</t>
   </si>
   <si>
     <t>96 of 6334 genes, 1.5%</t>
   </si>
   <si>
-    <t>PTC1,FCP1,PSY2</t>
-  </si>
-  <si>
     <t xml:space="preserve"> RNA binding</t>
   </si>
   <si>
     <t>756 of 6334 genes, 11.9%</t>
   </si>
   <si>
-    <t>NOP14,PRT1,MEX67</t>
-  </si>
-  <si>
     <t xml:space="preserve"> enzyme binding</t>
   </si>
   <si>
@@ -237,45 +180,30 @@
     <t>55 of 6334 genes, 0.9%</t>
   </si>
   <si>
-    <t>EXO70,CTR9</t>
-  </si>
-  <si>
     <t xml:space="preserve"> enzyme regulator activity</t>
   </si>
   <si>
     <t>223 of 6334 genes, 3.5%</t>
   </si>
   <si>
-    <t>SSE1,SEC23</t>
-  </si>
-  <si>
     <t xml:space="preserve"> nucleic acid binding transcription factor activity</t>
   </si>
   <si>
     <t>160 of 6334 genes, 2.5%</t>
   </si>
   <si>
-    <t>TAF5,BAS1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> unfolded protein binding</t>
   </si>
   <si>
     <t>67 of 6334 genes, 1.1%</t>
   </si>
   <si>
-    <t>ZUO1,HSC82</t>
-  </si>
-  <si>
     <t xml:space="preserve"> GTPase activity</t>
   </si>
   <si>
     <t>58 of 6334 genes, 0.9%</t>
   </si>
   <si>
-    <t>FZO1,NPA3</t>
-  </si>
-  <si>
     <t xml:space="preserve"> structural constituent of ribosome</t>
   </si>
   <si>
@@ -285,66 +213,42 @@
     <t>224 of 6334 genes, 3.5%</t>
   </si>
   <si>
-    <t>PET123</t>
-  </si>
-  <si>
     <t xml:space="preserve"> translation factor activity, nucleic acid binding</t>
   </si>
   <si>
     <t>45 of 6334 genes, 0.7%</t>
   </si>
   <si>
-    <t>PRT1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> hydrolase activity, acting on glycosyl bonds</t>
   </si>
   <si>
     <t>47 of 6334 genes, 0.7%</t>
   </si>
   <si>
-    <t>UNG1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> protein transporter activity</t>
   </si>
   <si>
     <t>52 of 6334 genes, 0.8%</t>
   </si>
   <si>
-    <t>TOM40</t>
-  </si>
-  <si>
     <t xml:space="preserve"> protein binding, bridging</t>
   </si>
   <si>
-    <t>RAD23</t>
-  </si>
-  <si>
     <t xml:space="preserve"> lipid binding</t>
   </si>
   <si>
     <t>95 of 6334 genes, 1.5%</t>
   </si>
   <si>
-    <t>EXO70</t>
-  </si>
-  <si>
     <t xml:space="preserve"> lyase activity</t>
   </si>
   <si>
-    <t>TRP2</t>
-  </si>
-  <si>
     <t xml:space="preserve"> nucleotidyltransferase activity</t>
   </si>
   <si>
     <t>114 of 6334 genes, 1.8%</t>
   </si>
   <si>
-    <t>PRI1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> cytoskeletal protein binding</t>
   </si>
   <si>
@@ -423,17 +327,204 @@
     <t>12 out of 106 genes, 11.3%</t>
   </si>
   <si>
-    <t>ACH1,FAP7,IPT1,VPS52,YND1,ARO9,SEC24,GFA1,DRE2,APL5,SRP72,TKL1</t>
+    <t>48,56,80,100</t>
+  </si>
+  <si>
+    <t>16,24,90</t>
+  </si>
+  <si>
+    <t>6,10,14,27,29,52,68,69,72,83,86,87,88</t>
+  </si>
+  <si>
+    <t>12,18,34</t>
+  </si>
+  <si>
+    <t>23,34,94</t>
+  </si>
+  <si>
+    <t>7,8,9</t>
+  </si>
+  <si>
+    <t>15,78,84</t>
+  </si>
+  <si>
+    <t>19,97,101</t>
+  </si>
+  <si>
+    <t>56,93</t>
+  </si>
+  <si>
+    <t>12,17,21,95,101</t>
+  </si>
+  <si>
+    <t>13,31,40,73,79</t>
+  </si>
+  <si>
+    <t>28,30,44,67,93</t>
+  </si>
+  <si>
+    <t>33,43,46,57,58</t>
+  </si>
+  <si>
+    <t>1,5,42,51,64,77</t>
+  </si>
+  <si>
+    <t>4,40,63,72,84,98</t>
+  </si>
+  <si>
+    <t>30,68,83,91,100,107</t>
+  </si>
+  <si>
+    <t>"RFA1","RAD23","PRI1","RFC2","BAS1","PMS1","ADE12","CTR9","HST3"</t>
+  </si>
+  <si>
+    <t>"ATP3","DBP10","CDC48","FAL1","RFC2","NPA3","HSC82","PMS1","DBP6"</t>
+  </si>
+  <si>
+    <t>"GDH2","ERG26","POX1","KGD1","ERG5","ARA2"</t>
+  </si>
+  <si>
+    <t>2,34,55,59,67,80,85,93,94</t>
+  </si>
+  <si>
+    <t>"CDC34","AIM10","VAS1","DED81","TRL1","TUL1","ADE12","GSH2","WRS1","MSD1"</t>
+  </si>
+  <si>
+    <t>25,36,45,49,57,62,85,91,92,99</t>
+  </si>
+  <si>
+    <t>5,16,18,24,59,60,76,80,90</t>
+  </si>
+  <si>
+    <t>22,39,41,54,74,75</t>
+  </si>
+  <si>
+    <t>"TOM40"</t>
+  </si>
+  <si>
+    <t>"PET123"</t>
+  </si>
+  <si>
+    <t>"EXO70"</t>
+  </si>
+  <si>
+    <t>"RAD23"</t>
+  </si>
+  <si>
+    <t>"PRT1"</t>
+  </si>
+  <si>
+    <t>"UNG1"</t>
+  </si>
+  <si>
+    <t>"TRP2"</t>
+  </si>
+  <si>
+    <t>"PRI1"</t>
+  </si>
+  <si>
+    <t>"NGG1","TGL4","LEU4","LRO1","ERG10","TAZ1"</t>
+  </si>
+  <si>
+    <t>"MAP2","DUG1","STE24","STE23","NMA111","MCA1"</t>
+  </si>
+  <si>
+    <t>"FLC2","ATP3","VRG4","AVT7","OAC1","TOM40"</t>
+  </si>
+  <si>
+    <t>"CAB1","HXK2","XKS1","TRL1","LSB6"</t>
+  </si>
+  <si>
+    <t>"NGG1","SSN2","TFG2","BAS1","CTR9"</t>
+  </si>
+  <si>
+    <t>"SPB1","RMT2","IME4","COQ5","GCD10"</t>
+  </si>
+  <si>
+    <t>"TAF5","NUP84","SEC31","PET123","MEX67"</t>
+  </si>
+  <si>
+    <t>"YLF2","EXO70","PMS1","SSE1"</t>
+  </si>
+  <si>
+    <t>"DBP10","FAL1","DBP6"</t>
+  </si>
+  <si>
+    <t>"TAF5","CDC48","RAD23"</t>
+  </si>
+  <si>
+    <t>"GUD1","RAD23","HST3"</t>
+  </si>
+  <si>
+    <t>"ALG14","ALG1","TPS1"</t>
+  </si>
+  <si>
+    <t>"PTC1","FCP1","PSY2"</t>
+  </si>
+  <si>
+    <t>"NOP14","PRT1","MEX67"</t>
+  </si>
+  <si>
+    <t>"EXO70","CTR9"</t>
+  </si>
+  <si>
+    <t>"SSE1","SEC23"</t>
+  </si>
+  <si>
+    <t>"TAF5","BAS1"</t>
+  </si>
+  <si>
+    <t>"ZUO1","HSC82"</t>
+  </si>
+  <si>
+    <t>"FZO1","NPA3"</t>
+  </si>
+  <si>
+    <t>"YBR056W","TOS1","CWH43","ARX1","BCP1","ICE2","FRA1","YLR253W","YML096W","YNL155W","RPA49","SEC21","EMW1"</t>
+  </si>
+  <si>
+    <t>"ACH1","FAP7","IPT1","VPS52","YND1","ARO9","SEC24","GFA1","DRE2","APL5","SRP72","TKL1"</t>
+  </si>
+  <si>
+    <t>12,67</t>
+  </si>
+  <si>
+    <t>47,76</t>
+  </si>
+  <si>
+    <t>11,60</t>
+  </si>
+  <si>
+    <t>3,20,26,32,35,50,53,63,65,102,103,104</t>
+  </si>
+  <si>
+    <t>order in rokas gene data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -456,13 +547,167 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="75">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -792,13 +1037,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="36.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="4" max="5" width="23.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -812,10 +1064,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>3674</v>
       </c>
@@ -829,739 +1084,839 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>16874</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>123</v>
+      </c>
+      <c r="F3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3677</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>121</v>
+      </c>
+      <c r="F4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>16887</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>16491</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>125</v>
+      </c>
+      <c r="F6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>16746</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>117</v>
+      </c>
+      <c r="F7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>8233</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>116</v>
+      </c>
+      <c r="F8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>22857</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>115</v>
+      </c>
+      <c r="F9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>16301</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>114</v>
+      </c>
+      <c r="F10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>988</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>113</v>
+      </c>
+      <c r="F11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>8168</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>112</v>
+      </c>
+      <c r="F12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>5198</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>111</v>
+      </c>
+      <c r="F13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>43167</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>102</v>
+      </c>
+      <c r="F14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>4386</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>103</v>
+      </c>
+      <c r="F15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>32182</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>105</v>
+      </c>
+      <c r="F16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>16810</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>106</v>
+      </c>
+      <c r="F17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>16757</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>107</v>
+      </c>
+      <c r="F18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>16791</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>108</v>
+      </c>
+      <c r="F19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>3723</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>109</v>
+      </c>
+      <c r="F20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>19899</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>110</v>
+      </c>
+      <c r="F21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>30234</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
-      </c>
-      <c r="E22" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>54</v>
+      </c>
+      <c r="E22" s="1">
+        <v>100106</v>
+      </c>
+      <c r="F22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>1071</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>155</v>
+      </c>
+      <c r="F23" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>51082</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="E24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>156</v>
+      </c>
+      <c r="F24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>3924</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>157</v>
+      </c>
+      <c r="F25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>3735</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="D26" t="s">
-        <v>87</v>
-      </c>
-      <c r="E26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>63</v>
+      </c>
+      <c r="E26" s="2">
+        <v>95</v>
+      </c>
+      <c r="F26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>8135</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>65</v>
+      </c>
+      <c r="E27" s="2">
+        <v>97</v>
+      </c>
+      <c r="F27" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>16798</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="D28" t="s">
-        <v>93</v>
-      </c>
-      <c r="E28" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>67</v>
+      </c>
+      <c r="E28" s="2">
+        <v>71</v>
+      </c>
+      <c r="F28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>8565</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="D29" t="s">
-        <v>96</v>
-      </c>
-      <c r="E29" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>69</v>
+      </c>
+      <c r="E29" s="2">
+        <v>77</v>
+      </c>
+      <c r="F29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>30674</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>65</v>
+      </c>
+      <c r="E30" s="2">
+        <v>34</v>
+      </c>
+      <c r="F30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>8289</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
-      </c>
-      <c r="E31" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>72</v>
+      </c>
+      <c r="E31" s="2">
+        <v>37</v>
+      </c>
+      <c r="F31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>16829</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>52</v>
-      </c>
-      <c r="E32" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>39</v>
+      </c>
+      <c r="E32" s="2">
+        <v>55</v>
+      </c>
+      <c r="F32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>16779</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="C33" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="D33" t="s">
-        <v>106</v>
-      </c>
-      <c r="E33" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>75</v>
+      </c>
+      <c r="E33" s="2">
+        <v>56</v>
+      </c>
+      <c r="F33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>8092</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="D34" t="s">
-        <v>110</v>
-      </c>
-      <c r="E34" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>78</v>
+      </c>
+      <c r="F34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>8134</v>
       </c>
       <c r="B35" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="C35" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="D35" t="s">
-        <v>113</v>
-      </c>
-      <c r="E35" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>81</v>
+      </c>
+      <c r="F35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>19843</v>
       </c>
       <c r="B36" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="D36" t="s">
-        <v>115</v>
-      </c>
-      <c r="E36" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>83</v>
+      </c>
+      <c r="F36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>16765</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="D37" t="s">
-        <v>117</v>
-      </c>
-      <c r="E37" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>85</v>
+      </c>
+      <c r="F37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>4871</v>
       </c>
       <c r="B38" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="D38" t="s">
-        <v>119</v>
-      </c>
-      <c r="E38" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>87</v>
+      </c>
+      <c r="F38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>30533</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="D39" t="s">
-        <v>121</v>
-      </c>
-      <c r="E39" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>89</v>
+      </c>
+      <c r="F39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>30555</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="D40" t="s">
-        <v>123</v>
-      </c>
-      <c r="E40" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>91</v>
+      </c>
+      <c r="F40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>16853</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
-      </c>
-      <c r="E41" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>93</v>
+      </c>
+      <c r="F41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>42393</v>
       </c>
       <c r="B42" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="C42" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="D42" t="s">
-        <v>127</v>
-      </c>
-      <c r="E42" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>95</v>
+      </c>
+      <c r="F42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>3729</v>
       </c>
       <c r="B43" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="C43" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="D43" t="s">
-        <v>129</v>
-      </c>
-      <c r="E43" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>97</v>
+      </c>
+      <c r="F43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>4518</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="C44" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="D44" t="s">
-        <v>131</v>
-      </c>
-      <c r="E44" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>99</v>
+      </c>
+      <c r="F44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="C45" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="E45" t="s">
-        <v>134</v>
+        <v>158</v>
+      </c>
+      <c r="F45" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>